<commit_message>
Added screen captures of the Excel-solution for problem 3, exercise 1.
</commit_message>
<xml_diff>
--- a/exercise-1/Exercise-set-1, task 3.xlsx
+++ b/exercise-1/Exercise-set-1, task 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/johannvk_ntnu_no/Documents/FYSMAT/Høst 2021/Operations-Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/johannvk_ntnu_no/Documents/FYSMAT/Høst 2021/Operations-Analysis/TIOE4120-Operational-analysis-H21/exercise-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="678" documentId="8_{BCB3EB48-C005-4F37-84B3-9951538216E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7981AA06-68DD-4D9C-8A20-93D8887F55DA}"/>
+  <xr:revisionPtr revIDLastSave="695" documentId="8_{BCB3EB48-C005-4F37-84B3-9951538216E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B400C77-AD1F-435E-AB76-BEEDCED76295}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{80D87421-A8B3-4C76-BBA0-3537348AFD70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{80D87421-A8B3-4C76-BBA0-3537348AFD70}"/>
   </bookViews>
   <sheets>
     <sheet name="Answer Report 2" sheetId="5" r:id="rId1"/>
@@ -624,15 +624,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,6 +649,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,50 +988,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1051,30 +1051,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="16">
         <v>0</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="16">
         <v>300</v>
       </c>
     </row>
@@ -1084,70 +1084,70 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="17">
         <v>0</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="17">
         <v>100</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="17">
         <v>0</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="17">
         <v>200</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="16">
         <v>0</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="16">
         <v>0</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1157,82 +1157,82 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="17">
         <v>400</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="17">
         <v>150</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="20">
+      <c r="G29" s="17">
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="16">
         <v>300</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1260,17 +1260,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1280,113 +1280,113 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="15">
         <v>100</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="15">
         <v>0</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="15">
         <v>1</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="15">
         <v>1</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="15">
         <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="15">
         <v>200</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="15">
         <v>0</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="15">
         <v>1</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="15">
         <v>6.25E-2</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="15">
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>0</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="13">
         <v>1</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="13">
         <v>1E+30</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -1396,113 +1396,113 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="15">
         <v>400</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="15">
         <v>0.5</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="15">
         <v>400</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="15">
         <v>1E+30</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="15">
         <v>200</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <v>150</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="15">
         <v>0</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="15">
         <v>100</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="15">
         <v>50</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="15">
         <v>1E+30</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="13">
         <v>300</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="13">
         <v>300</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="13">
         <v>300</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="13">
         <v>299.99999999999994</v>
       </c>
     </row>
@@ -1532,159 +1532,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="21"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="16">
         <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="F11" s="21" t="s">
+      <c r="D11" s="18"/>
+      <c r="F11" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="17">
         <v>100</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="17">
         <v>100</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="17">
         <v>300</v>
       </c>
-      <c r="I13" s="18" t="e">
+      <c r="I13" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J13" s="18" t="e">
+      <c r="J13" s="15" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="17">
         <v>200</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="17">
         <v>200</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="17">
         <v>300</v>
       </c>
-      <c r="I14" s="18" t="e">
+      <c r="I14" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J14" s="18" t="e">
+      <c r="J14" s="15" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="16">
         <v>0</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="16">
         <v>0</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <v>300</v>
       </c>
-      <c r="I15" s="16" t="e">
+      <c r="I15" s="13" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J15" s="16" t="e">
+      <c r="J15" s="13" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,11 +1708,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1738,25 +1738,25 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="11">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="25"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1766,10 +1766,10 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="27"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1789,10 +1789,10 @@
         <v>6</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="27"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="26">
+      <c r="B10" s="23">
         <v>5</v>
       </c>
       <c r="C10" s="3">
@@ -1815,10 +1815,10 @@
         <v>400</v>
       </c>
       <c r="I10" s="7"/>
-      <c r="J10" s="27"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="26">
+      <c r="B11" s="23">
         <v>10</v>
       </c>
       <c r="C11" s="6">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="F11" s="7">
         <f t="shared" ref="F11:F12" si="0">$D$3*C11+$D$4*D11+$D$5*E11</f>
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>12</v>
@@ -1841,33 +1841,33 @@
         <v>100</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="27"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="28">
+      <c r="B12" s="25">
         <v>20</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="27">
         <v>1.5</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="28">
         <v>2</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="29">
         <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="29">
         <v>300</v>
       </c>
-      <c r="G12" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="32">
-        <v>300</v>
-      </c>
-      <c r="I12" s="32"/>
-      <c r="J12" s="33"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="C15" s="2">
         <f>D3+D4+D5</f>
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to the excel file.
</commit_message>
<xml_diff>
--- a/exercise-1/Exercise-set-1, task 3.xlsx
+++ b/exercise-1/Exercise-set-1, task 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/johannvk_ntnu_no/Documents/FYSMAT/Høst 2021/Operations-Analysis/TIOE4120-Operational-analysis-H21/exercise-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="8_{BCB3EB48-C005-4F37-84B3-9951538216E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B400C77-AD1F-435E-AB76-BEEDCED76295}"/>
+  <xr:revisionPtr revIDLastSave="704" documentId="8_{BCB3EB48-C005-4F37-84B3-9951538216E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C344CDE7-B172-4196-9E94-DA11FBF7AAF1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{80D87421-A8B3-4C76-BBA0-3537348AFD70}"/>
   </bookViews>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5">
-        <v>80</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8">
-        <v>200</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="F10" s="7">
         <f>$D$3*C10+$D$4*D10+$D$5*E10</f>
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>12</v>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="F11" s="7">
         <f t="shared" ref="F11:F12" si="0">$D$3*C11+$D$4*D11+$D$5*E11</f>
-        <v>220</v>
+        <v>194.5</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>12</v>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="F12" s="29">
         <f t="shared" si="0"/>
-        <v>460</v>
+        <v>301</v>
       </c>
       <c r="G12" s="29" t="s">
         <v>12</v>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="C15" s="2">
         <f>D3+D4+D5</f>
-        <v>360</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>